<commit_message>
Modified factor value code to conform to new template.
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/gus/GusAppFramework/branches/4.0@12996 4235af6a-31f9-0310-9ad3-ecf6348f2534
</commit_message>
<xml_diff>
--- a/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx5.xlsx
+++ b/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-7635" yWindow="2415" windowWidth="19440" windowHeight="8085" tabRatio="162" activeTab="1"/>
@@ -944,7 +944,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="41">
     <font>
       <sz val="11"/>
@@ -1953,7 +1953,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1988,7 +1987,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2164,11 +2162,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV61"/>
   <sheetViews>
-    <sheetView topLeftCell="I41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2203,7 +2201,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60">
+    <row r="3" spans="1:10">
       <c r="A3" s="70" t="s">
         <v>12</v>
       </c>
@@ -4348,11 +4346,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BT2" sqref="BT2:BT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4826,7 +4824,7 @@
       <c r="BS2" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BT2" s="53" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5298,7 +5296,7 @@
       <c r="BS4" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="BT4" s="4" t="s">
+      <c r="BT4" s="53" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5503,7 +5501,7 @@
       <c r="BS5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="BT5" s="4" t="s">
+      <c r="BT5" s="53" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5710,7 +5708,7 @@
       <c r="BS6" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="BT6" s="4" t="s">
+      <c r="BT6" s="53" t="s">
         <v>266</v>
       </c>
     </row>
@@ -5917,7 +5915,7 @@
       <c r="BS7" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="BT7" s="4" t="s">
+      <c r="BT7" s="53" t="s">
         <v>266</v>
       </c>
     </row>
@@ -6129,7 +6127,7 @@
       <c r="BS8" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="BT8" s="4" t="s">
+      <c r="BT8" s="53" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>